<commit_message>
Add PM species tables to appendix
</commit_message>
<xml_diff>
--- a/outputs/chemical composition tables.xlsx
+++ b/outputs/chemical composition tables.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://colostate-my.sharepoint.com/personal/emcarter_colostate_edu/Documents/Active Research/BHET/Admin/Final Report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samharper/git/bhet-report/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{81229809-75CF-3D4C-B6B5-0A8AE5DC38D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C254A55-4551-BF4C-A1C6-1F3B9DF22685}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105BF5E3-27ED-4D48-8F5A-B8BA472D93EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6800" yWindow="880" windowWidth="22340" windowHeight="17440" xr2:uid="{401DA6FC-8AD3-4941-BE38-CE13CA5C5C54}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="outdoor" sheetId="1" r:id="rId1"/>
+    <sheet name="personal" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="129">
-  <si>
-    <t>Outdoor</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="127">
   <si>
     <t>wave</t>
   </si>
@@ -417,9 +415,6 @@
   </si>
   <si>
     <t>2.06 (1.81-2.3)</t>
-  </si>
-  <si>
-    <t>Personal exposure</t>
   </si>
   <si>
     <t>8.75 (8.36-9.14)</t>
@@ -801,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8F6A79-7A37-CC46-B62D-3D0295152990}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A1:XFD16"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -828,574 +823,494 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>2</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA95F9B-B79B-BE4C-AC9D-ADCF5312F147}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>